<commit_message>
test: add another approach in test.py
</commit_message>
<xml_diff>
--- a/source.xlsx
+++ b/source.xlsx
@@ -119,12 +119,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,42 +323,42 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>